<commit_message>
Added npc searching for shopping list items and either leaving or finding items, next going to the checkout to buy items
</commit_message>
<xml_diff>
--- a/Games/GuildManagerFolder/GuildManager2d/CSV/shop_item.xlsx
+++ b/Games/GuildManagerFolder/GuildManager2d/CSV/shop_item.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\GodotProjects\Games\GuildManagerFolder\GuildManager2d\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69041D15-4A90-4E4B-82E4-E0A795EC03DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2A59F7-6106-4757-9382-802B9AE66CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25490" yWindow="3460" windowWidth="19420" windowHeight="10560" xr2:uid="{6613D835-19EA-40EE-98A1-1D2837994A45}"/>
   </bookViews>
@@ -1054,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97A1F4D6-F08C-4BFA-8F0D-CD932C622A30}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,7 +1122,8 @@
         <v>5</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <f>ROUND(E2 * 1.2,0)</f>
+        <v>6</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -1131,6 +1132,9 @@
         <v>9</v>
       </c>
       <c r="I2">
+        <v>20</v>
+      </c>
+      <c r="J2">
         <v>20</v>
       </c>
       <c r="K2">
@@ -1156,6 +1160,7 @@
         <v>10</v>
       </c>
       <c r="F3">
+        <f t="shared" ref="F3:F21" si="0">ROUND(E3 * 1.2,0)</f>
         <v>12</v>
       </c>
       <c r="G3">
@@ -1167,6 +1172,9 @@
       <c r="I3">
         <v>15</v>
       </c>
+      <c r="J3">
+        <v>15</v>
+      </c>
       <c r="K3">
         <v>30</v>
       </c>
@@ -1174,7 +1182,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A21" si="0">A3+1</f>
+        <f t="shared" ref="A4:A21" si="1">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -1190,7 +1198,8 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1201,6 +1210,9 @@
       <c r="I4">
         <v>50</v>
       </c>
+      <c r="J4">
+        <v>50</v>
+      </c>
       <c r="K4">
         <v>100</v>
       </c>
@@ -1208,7 +1220,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -1224,7 +1236,8 @@
         <v>8</v>
       </c>
       <c r="F5">
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -1235,6 +1248,9 @@
       <c r="I5">
         <v>10</v>
       </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
       <c r="K5">
         <v>20</v>
       </c>
@@ -1242,7 +1258,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -1258,7 +1274,8 @@
         <v>30</v>
       </c>
       <c r="F6">
-        <v>28</v>
+        <f t="shared" si="0"/>
+        <v>36</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1266,433 +1283,492 @@
       <c r="I6">
         <v>5</v>
       </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
       <c r="K6">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7">
+        <v>120</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8">
+        <v>25</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>8</v>
+      </c>
+      <c r="J8">
+        <v>8</v>
+      </c>
+      <c r="K8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>40</v>
+      </c>
+      <c r="J9">
+        <v>40</v>
+      </c>
+      <c r="K9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10">
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>25</v>
+      </c>
+      <c r="J11">
+        <v>25</v>
+      </c>
+      <c r="K11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7">
-        <v>120</v>
-      </c>
-      <c r="F7">
-        <v>110</v>
-      </c>
-      <c r="G7">
+      <c r="G12">
         <v>0</v>
       </c>
-      <c r="I7">
-        <v>2</v>
-      </c>
-      <c r="K7">
+      <c r="I12">
+        <v>40</v>
+      </c>
+      <c r="J12">
+        <v>40</v>
+      </c>
+      <c r="K12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>9</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>30</v>
+      </c>
+      <c r="J13">
+        <v>30</v>
+      </c>
+      <c r="K13">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>10</v>
+      </c>
+      <c r="J14">
+        <v>10</v>
+      </c>
+      <c r="K14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15">
+        <v>50</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="I15">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="J15">
+        <v>5</v>
+      </c>
+      <c r="K15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>60</v>
+      </c>
+      <c r="J16">
+        <v>60</v>
+      </c>
+      <c r="K16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17">
+        <v>80</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18">
         <v>30</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>8</v>
+      </c>
+      <c r="J18">
+        <v>8</v>
+      </c>
+      <c r="K18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
         <v>31</v>
       </c>
-      <c r="E8">
-        <v>25</v>
-      </c>
-      <c r="F8">
-        <v>23</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="I8">
+      <c r="E19">
         <v>8</v>
       </c>
-      <c r="K8">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9">
-        <v>7</v>
-      </c>
-      <c r="F9">
-        <v>6</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>40</v>
-      </c>
-      <c r="K9">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10">
-        <v>50</v>
-      </c>
-      <c r="F10">
-        <v>48</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>4</v>
-      </c>
-      <c r="K10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11">
-        <v>12</v>
-      </c>
-      <c r="F11">
-        <v>11</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>25</v>
-      </c>
-      <c r="K11">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="F19">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>30</v>
+      </c>
+      <c r="J19">
+        <v>30</v>
+      </c>
+      <c r="K19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
         <v>40</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D20" t="s">
         <v>34</v>
       </c>
-      <c r="E12">
-        <v>4</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>40</v>
-      </c>
-      <c r="K12">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13">
-        <v>9</v>
-      </c>
-      <c r="F13">
-        <v>8</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>30</v>
-      </c>
-      <c r="K13">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f t="shared" si="0"/>
+      <c r="E20">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14">
-        <v>15</v>
-      </c>
-      <c r="F14">
-        <v>14</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>10</v>
-      </c>
-      <c r="K14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15">
-        <v>50</v>
-      </c>
-      <c r="F15">
-        <v>52</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>5</v>
-      </c>
-      <c r="K15">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="F20">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16">
-        <v>5</v>
-      </c>
-      <c r="F16">
-        <v>6</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>60</v>
-      </c>
-      <c r="K16">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17">
-        <v>80</v>
-      </c>
-      <c r="F17">
-        <v>75</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>3</v>
-      </c>
-      <c r="K17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18">
-        <v>30</v>
-      </c>
-      <c r="F18">
-        <v>28</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>8</v>
-      </c>
-      <c r="K18">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19">
-        <v>8</v>
-      </c>
-      <c r="F19">
-        <v>9</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>30</v>
-      </c>
-      <c r="K19">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20">
-        <v>12</v>
-      </c>
-      <c r="F20">
-        <v>11</v>
-      </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="I20">
         <v>20</v>
       </c>
+      <c r="J20">
+        <v>20</v>
+      </c>
       <c r="K20">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B21" t="s">
@@ -1708,12 +1784,16 @@
         <v>5</v>
       </c>
       <c r="F21">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="I21">
+        <v>50</v>
+      </c>
+      <c r="J21">
         <v>50</v>
       </c>
       <c r="K21">

</xml_diff>